<commit_message>
adapt calculation for Resistor R1,R2,R4 from 1310Ohm to 1298Ohm
</commit_message>
<xml_diff>
--- a/tools/PT1000_lookup_table.xlsx
+++ b/tools/PT1000_lookup_table.xlsx
@@ -32,6 +32,7 @@
             <sz val="10"/>
             <rFont val="Arial"/>
             <family val="2"/>
+            <charset val="1"/>
           </rPr>
           <t xml:space="preserve">Bei GANE 8
 1 Bit = 0,25 mV</t>
@@ -45,6 +46,7 @@
             <sz val="10"/>
             <rFont val="Arial"/>
             <family val="2"/>
+            <charset val="1"/>
           </rPr>
           <t xml:space="preserve">T_calc = m*Um+b</t>
         </r>
@@ -108,11 +110,12 @@
     <numFmt numFmtId="165" formatCode="0.00"/>
     <numFmt numFmtId="166" formatCode="General"/>
   </numFmts>
-  <fonts count="5">
+  <fonts count="6">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -131,6 +134,12 @@
     </font>
     <font>
       <b val="true"/>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
@@ -190,7 +199,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="9">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -220,10 +229,6 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -303,7 +308,7 @@
 </styleSheet>
 </file>
 
-<file path=xl/charts/chart7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -315,10 +320,10 @@
           <c:layoutTarget val="inner"/>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.0340828095639215"/>
-          <c:y val="0.0377570416450665"/>
-          <c:w val="0.870990734141126"/>
-          <c:h val="0.93675479523069"/>
+          <c:x val="0.0340928270042194"/>
+          <c:y val="0.0377460858781584"/>
+          <c:w val="0.870942334739803"/>
+          <c:h val="0.936676484266005"/>
         </c:manualLayout>
       </c:layout>
       <c:scatterChart>
@@ -356,6 +361,7 @@
                 </a:pPr>
               </a:p>
             </c:txPr>
+            <c:dLblPos val="r"/>
             <c:showLegendKey val="0"/>
             <c:showVal val="0"/>
             <c:showCatName val="0"/>
@@ -451,87 +457,87 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="22"/>
                 <c:pt idx="0">
-                  <c:v>1583</c:v>
+                  <c:v>1554</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1432</c:v>
+                  <c:v>1403</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1287</c:v>
+                  <c:v>1258</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1148</c:v>
+                  <c:v>1119</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>1014</c:v>
+                  <c:v>984</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>885</c:v>
+                  <c:v>855</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>761</c:v>
+                  <c:v>731</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>641</c:v>
+                  <c:v>611</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>582</c:v>
+                  <c:v>552</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>525</c:v>
+                  <c:v>495</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>413</c:v>
+                  <c:v>383</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>305</c:v>
+                  <c:v>275</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>201</c:v>
+                  <c:v>171</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>100</c:v>
+                  <c:v>70</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>2</c:v>
+                  <c:v>-28</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>-92</c:v>
+                  <c:v>-123</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>-184</c:v>
+                  <c:v>-215</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>-273</c:v>
+                  <c:v>-303</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>-359</c:v>
+                  <c:v>-390</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>-443</c:v>
+                  <c:v>-473</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>-524</c:v>
+                  <c:v>-554</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>-603</c:v>
+                  <c:v>-633</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:yVal>
           <c:smooth val="0"/>
         </c:ser>
-        <c:axId val="61933892"/>
-        <c:axId val="61354668"/>
+        <c:axId val="94259597"/>
+        <c:axId val="92477654"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="61933892"/>
+        <c:axId val="94259597"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:numFmt formatCode="General" sourceLinked="0"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -553,12 +559,12 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="61354668"/>
+        <c:crossAx val="92477654"/>
         <c:crosses val="autoZero"/>
-        <c:crossBetween val="between"/>
+        <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="61354668"/>
+        <c:axId val="92477654"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -573,7 +579,7 @@
             </a:ln>
           </c:spPr>
         </c:majorGridlines>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:numFmt formatCode="General" sourceLinked="0"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -595,9 +601,9 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="61933892"/>
+        <c:crossAx val="94259597"/>
         <c:crosses val="autoZero"/>
-        <c:crossBetween val="between"/>
+        <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:spPr>
         <a:noFill/>
@@ -654,9 +660,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>18</xdr:col>
-      <xdr:colOff>283320</xdr:colOff>
+      <xdr:colOff>282960</xdr:colOff>
       <xdr:row>33</xdr:row>
-      <xdr:rowOff>100800</xdr:rowOff>
+      <xdr:rowOff>100440</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -664,8 +670,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="8475480" y="820440"/>
-        <a:ext cx="6389280" cy="4644720"/>
+        <a:off x="8487720" y="820440"/>
+        <a:ext cx="6398640" cy="4644360"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -686,12 +692,12 @@
   <dimension ref="A1:J25"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C25" activeCellId="0" sqref="C25"/>
+      <selection pane="topLeft" activeCell="C12" activeCellId="0" sqref="C12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="10.83"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="10.84"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -705,19 +711,19 @@
         <v>1</v>
       </c>
       <c r="D1" s="2" t="n">
-        <v>1310</v>
+        <v>1298</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>2</v>
       </c>
       <c r="F1" s="2" t="n">
-        <v>1310</v>
+        <v>1298</v>
       </c>
       <c r="G1" s="1" t="s">
         <v>3</v>
       </c>
       <c r="H1" s="2" t="n">
-        <v>1310</v>
+        <v>1298</v>
       </c>
       <c r="I1" s="1" t="s">
         <v>4</v>
@@ -761,11 +767,11 @@
       </c>
       <c r="C4" s="3" t="n">
         <f aca="false">$B$1*($D$1*$H$1-B4*$F$1)/(($D$1+$F$1)*(B4+$H$1))*1000</f>
-        <v>395.809474232171</v>
+        <v>388.64642330208</v>
       </c>
       <c r="D4" s="0" t="n">
         <f aca="false">INT(C4/$J$1)</f>
-        <v>1583</v>
+        <v>1554</v>
       </c>
       <c r="E4" s="0" t="s">
         <v>13</v>
@@ -783,11 +789,11 @@
       </c>
       <c r="C5" s="3" t="n">
         <f aca="false">$B$1*($D$1*$H$1-B5*$F$1)/(($D$1+$F$1)*(B5+$H$1))*1000</f>
-        <v>358.17577925396</v>
+        <v>350.934273835661</v>
       </c>
       <c r="D5" s="0" t="n">
         <f aca="false">INT(C5/$J$1)</f>
-        <v>1432</v>
+        <v>1403</v>
       </c>
       <c r="E5" s="0" t="s">
         <v>13</v>
@@ -805,11 +811,11 @@
       </c>
       <c r="C6" s="3" t="n">
         <f aca="false">$B$1*($D$1*$H$1-B6*$F$1)/(($D$1+$F$1)*(B6+$H$1))*1000</f>
-        <v>321.991606605237</v>
+        <v>314.682139253279</v>
       </c>
       <c r="D6" s="0" t="n">
         <f aca="false">INT(C6/$J$1)</f>
-        <v>1287</v>
+        <v>1258</v>
       </c>
       <c r="E6" s="0" t="s">
         <v>13</v>
@@ -827,11 +833,11 @@
       </c>
       <c r="C7" s="3" t="n">
         <f aca="false">$B$1*($D$1*$H$1-B7*$F$1)/(($D$1+$F$1)*(B7+$H$1))*1000</f>
-        <v>287.175120989425</v>
+        <v>279.807172463507</v>
       </c>
       <c r="D7" s="0" t="n">
         <f aca="false">INT(C7/$J$1)</f>
-        <v>1148</v>
+        <v>1119</v>
       </c>
       <c r="E7" s="0" t="s">
         <v>13</v>
@@ -849,11 +855,11 @@
       </c>
       <c r="C8" s="3" t="n">
         <f aca="false">$B$1*($D$1*$H$1-B8*$F$1)/(($D$1+$F$1)*(B8+$H$1))*1000</f>
-        <v>253.650535030164</v>
+        <v>246.232679622825</v>
       </c>
       <c r="D8" s="0" t="n">
         <f aca="false">INT(C8/$J$1)</f>
-        <v>1014</v>
+        <v>984</v>
       </c>
       <c r="E8" s="0" t="s">
         <v>13</v>
@@ -871,11 +877,11 @@
       </c>
       <c r="C9" s="3" t="n">
         <f aca="false">$B$1*($D$1*$H$1-B9*$F$1)/(($D$1+$F$1)*(B9+$H$1))*1000</f>
-        <v>221.428571428571</v>
+        <v>213.968668407311</v>
       </c>
       <c r="D9" s="5" t="n">
         <f aca="false">INT(C9/$J$1)</f>
-        <v>885</v>
+        <v>855</v>
       </c>
       <c r="E9" s="6" t="n">
         <f aca="false">($A$15-$A$9)/($D$15-$D$9)</f>
@@ -883,7 +889,7 @@
       </c>
       <c r="F9" s="6" t="n">
         <f aca="false">$A$9-E9*$D$9</f>
-        <v>76.2931034482759</v>
+        <v>73.7068965517241</v>
       </c>
       <c r="G9" s="0" t="n">
         <f aca="false">D9*E9+F9</f>
@@ -903,11 +909,11 @@
       </c>
       <c r="C10" s="3" t="n">
         <f aca="false">$B$1*($D$1*$H$1-B10*$F$1)/(($D$1+$F$1)*(B10+$H$1))*1000</f>
-        <v>190.357598978289</v>
+        <v>182.862644415918</v>
       </c>
       <c r="D10" s="0" t="n">
         <f aca="false">INT(C10/$J$1)</f>
-        <v>761</v>
+        <v>731</v>
       </c>
       <c r="E10" s="6" t="n">
         <f aca="false">($A$15-$A$9)/($D$15-$D$9)</f>
@@ -915,7 +921,7 @@
       </c>
       <c r="F10" s="6" t="n">
         <f aca="false">$A$9-E10*$D$9</f>
-        <v>76.2931034482759</v>
+        <v>73.7068965517241</v>
       </c>
       <c r="G10" s="0" t="n">
         <f aca="false">D10*E10+F10</f>
@@ -935,11 +941,11 @@
       </c>
       <c r="C11" s="3" t="n">
         <f aca="false">$B$1*($D$1*$H$1-B11*$F$1)/(($D$1+$F$1)*(B11+$H$1))*1000</f>
-        <v>160.377318983207</v>
+        <v>152.853655456879</v>
       </c>
       <c r="D11" s="0" t="n">
         <f aca="false">INT(C11/$J$1)</f>
-        <v>641</v>
+        <v>611</v>
       </c>
       <c r="E11" s="6" t="n">
         <f aca="false">($A$15-$A$9)/($D$15-$D$9)</f>
@@ -947,7 +953,7 @@
       </c>
       <c r="F11" s="6" t="n">
         <f aca="false">$A$9-E11*$D$9</f>
-        <v>76.2931034482759</v>
+        <v>73.7068965517241</v>
       </c>
       <c r="G11" s="0" t="n">
         <f aca="false">D11*E11+F11</f>
@@ -955,7 +961,7 @@
       </c>
       <c r="H11" s="0" t="n">
         <f aca="false">G11-A11</f>
-        <v>1.0344827586207</v>
+        <v>1.03448275862069</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -967,11 +973,11 @@
       </c>
       <c r="C12" s="3" t="n">
         <f aca="false">$B$1*($D$1*$H$1-B12*$F$1)/(($D$1+$F$1)*(B12+$H$1))*1000</f>
-        <v>145.713217579131</v>
+        <v>138.177339901478</v>
       </c>
       <c r="D12" s="0" t="n">
         <f aca="false">INT(C12/$J$1)</f>
-        <v>582</v>
+        <v>552</v>
       </c>
       <c r="E12" s="6" t="n">
         <f aca="false">($A$15-$A$9)/($D$15-$D$9)</f>
@@ -979,7 +985,7 @@
       </c>
       <c r="F12" s="6" t="n">
         <f aca="false">$A$9-E12*$D$9</f>
-        <v>76.2931034482759</v>
+        <v>73.7068965517241</v>
       </c>
       <c r="G12" s="0" t="n">
         <f aca="false">D12*E12+F12</f>
@@ -987,7 +993,7 @@
       </c>
       <c r="H12" s="0" t="n">
         <f aca="false">G12-A12</f>
-        <v>1.12068965517242</v>
+        <v>1.12068965517241</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -999,11 +1005,11 @@
       </c>
       <c r="C13" s="3" t="n">
         <f aca="false">$B$1*($D$1*$H$1-B13*$F$1)/(($D$1+$F$1)*(B13+$H$1))*1000</f>
-        <v>131.431573742119</v>
+        <v>123.884954652752</v>
       </c>
       <c r="D13" s="0" t="n">
         <f aca="false">INT(C13/$J$1)</f>
-        <v>525</v>
+        <v>495</v>
       </c>
       <c r="E13" s="6" t="n">
         <f aca="false">($A$15-$A$9)/($D$15-$D$9)</f>
@@ -1011,7 +1017,7 @@
       </c>
       <c r="F13" s="6" t="n">
         <f aca="false">$A$9-E13*$D$9</f>
-        <v>76.2931034482759</v>
+        <v>73.7068965517241</v>
       </c>
       <c r="G13" s="0" t="n">
         <f aca="false">D13*E13+F13</f>
@@ -1019,7 +1025,7 @@
       </c>
       <c r="H13" s="0" t="n">
         <f aca="false">G13-A13</f>
-        <v>1.0344827586207</v>
+        <v>1.03448275862069</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1031,11 +1037,11 @@
       </c>
       <c r="C14" s="3" t="n">
         <f aca="false">$B$1*($D$1*$H$1-B14*$F$1)/(($D$1+$F$1)*(B14+$H$1))*1000</f>
-        <v>103.467997079581</v>
+        <v>95.9036439227194</v>
       </c>
       <c r="D14" s="0" t="n">
         <f aca="false">INT(C14/$J$1)</f>
-        <v>413</v>
+        <v>383</v>
       </c>
       <c r="E14" s="6" t="n">
         <f aca="false">($A$15-$A$9)/($D$15-$D$9)</f>
@@ -1043,7 +1049,7 @@
       </c>
       <c r="F14" s="6" t="n">
         <f aca="false">$A$9-E14*$D$9</f>
-        <v>76.2931034482759</v>
+        <v>73.7068965517241</v>
       </c>
       <c r="G14" s="0" t="n">
         <f aca="false">D14*E14+F14</f>
@@ -1051,7 +1057,7 @@
       </c>
       <c r="H14" s="0" t="n">
         <f aca="false">G14-A14</f>
-        <v>0.689655172413801</v>
+        <v>0.689655172413794</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1063,11 +1069,11 @@
       </c>
       <c r="C15" s="3" t="n">
         <f aca="false">$B$1*($D$1*$H$1-B15*$F$1)/(($D$1+$F$1)*(B15+$H$1))*1000</f>
-        <v>76.4376996805112</v>
+        <v>68.8603531300161</v>
       </c>
       <c r="D15" s="5" t="n">
         <f aca="false">INT(C15/$J$1)</f>
-        <v>305</v>
+        <v>275</v>
       </c>
       <c r="E15" s="6" t="n">
         <f aca="false">($A$15-$A$9)/($D$15-$D$9)</f>
@@ -1075,7 +1081,7 @@
       </c>
       <c r="F15" s="6" t="n">
         <f aca="false">$A$9-E15*$D$9</f>
-        <v>76.2931034482759</v>
+        <v>73.7068965517241</v>
       </c>
       <c r="G15" s="0" t="n">
         <f aca="false">D15*E15+F15</f>
@@ -1087,7 +1093,7 @@
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="8" t="n">
+      <c r="A16" s="2" t="n">
         <v>60</v>
       </c>
       <c r="B16" s="0" t="n">
@@ -1095,11 +1101,11 @@
       </c>
       <c r="C16" s="3" t="n">
         <f aca="false">$B$1*($D$1*$H$1-B16*$F$1)/(($D$1+$F$1)*(B16+$H$1))*1000</f>
-        <v>50.3618628067966</v>
+        <v>42.7758457160922</v>
       </c>
       <c r="D16" s="0" t="n">
         <f aca="false">INT(C16/$J$1)</f>
-        <v>201</v>
+        <v>171</v>
       </c>
       <c r="E16" s="0" t="n">
         <f aca="false">($A$17-$A$15)/($D$17-$D$15)</f>
@@ -1107,7 +1113,7 @@
       </c>
       <c r="F16" s="0" t="n">
         <f aca="false">$A$15-E16*$D$15</f>
-        <v>79.7560975609756</v>
+        <v>76.8292682926829</v>
       </c>
       <c r="G16" s="0" t="n">
         <f aca="false">D16*E16+F16</f>
@@ -1127,11 +1133,11 @@
       </c>
       <c r="C17" s="3" t="n">
         <f aca="false">$B$1*($D$1*$H$1-B17*$F$1)/(($D$1+$F$1)*(B17+$H$1))*1000</f>
-        <v>25.1269035532995</v>
+        <v>17.5361077587884</v>
       </c>
       <c r="D17" s="5" t="n">
         <f aca="false">INT(C17/$J$1)</f>
-        <v>100</v>
+        <v>70</v>
       </c>
       <c r="E17" s="0" t="n">
         <f aca="false">($A$17-$A$15)/($D$17-$D$15)</f>
@@ -1139,7 +1145,7 @@
       </c>
       <c r="F17" s="0" t="n">
         <f aca="false">$A$15-E17*$D$15</f>
-        <v>79.7560975609756</v>
+        <v>76.8292682926829</v>
       </c>
       <c r="G17" s="0" t="n">
         <f aca="false">D17*E17+F17</f>
@@ -1151,7 +1157,7 @@
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="8" t="n">
+      <c r="A18" s="2" t="n">
         <v>80</v>
       </c>
       <c r="B18" s="0" t="n">
@@ -1159,27 +1165,27 @@
       </c>
       <c r="C18" s="3" t="n">
         <f aca="false">$B$1*($D$1*$H$1-B18*$F$1)/(($D$1+$F$1)*(B18+$H$1))*1000</f>
-        <v>0.693039062201576</v>
+        <v>-6.89899881084822</v>
       </c>
       <c r="D18" s="0" t="n">
         <f aca="false">INT(C18/$J$1)</f>
-        <v>2</v>
+        <v>-28</v>
       </c>
       <c r="E18" s="6" t="n">
         <f aca="false">($A$19-$A$17)/($D$19-$D$17)</f>
-        <v>-0.104166666666667</v>
+        <v>-0.103626943005181</v>
       </c>
       <c r="F18" s="6" t="n">
         <f aca="false">$A$17-E18*$D$17</f>
-        <v>80.4166666666667</v>
+        <v>77.2538860103627</v>
       </c>
       <c r="G18" s="0" t="n">
         <f aca="false">D18*E18+F18</f>
-        <v>80.2083333333333</v>
+        <v>80.1554404145078</v>
       </c>
       <c r="H18" s="0" t="n">
         <f aca="false">G18-A18</f>
-        <v>0.208333333333343</v>
+        <v>0.155440414507765</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1191,19 +1197,19 @@
       </c>
       <c r="C19" s="3" t="n">
         <f aca="false">$B$1*($D$1*$H$1-B19*$F$1)/(($D$1+$F$1)*(B19+$H$1))*1000</f>
-        <v>-22.9770417764396</v>
+        <v>-30.5671077504726</v>
       </c>
       <c r="D19" s="5" t="n">
         <f aca="false">INT(C19/$J$1)</f>
-        <v>-92</v>
+        <v>-123</v>
       </c>
       <c r="E19" s="6" t="n">
         <f aca="false">($A$19-$A$17)/($D$19-$D$17)</f>
-        <v>-0.104166666666667</v>
+        <v>-0.103626943005181</v>
       </c>
       <c r="F19" s="6" t="n">
         <f aca="false">$A$17-E19*$D$17</f>
-        <v>80.4166666666667</v>
+        <v>77.2538860103627</v>
       </c>
       <c r="G19" s="0" t="n">
         <f aca="false">D19*E19+F19</f>
@@ -1223,19 +1229,19 @@
       </c>
       <c r="C20" s="3" t="n">
         <f aca="false">$B$1*($D$1*$H$1-B20*$F$1)/(($D$1+$F$1)*(B20+$H$1))*1000</f>
-        <v>-45.9183673469388</v>
+        <v>-53.5035408125233</v>
       </c>
       <c r="D20" s="5" t="n">
         <f aca="false">INT(C20/$J$1)</f>
-        <v>-184</v>
-      </c>
-      <c r="E20" s="9" t="n">
+        <v>-215</v>
+      </c>
+      <c r="E20" s="8" t="n">
         <f aca="false">($A$20-$A$19)/($D$20-$D$19)</f>
         <v>-0.108695652173913</v>
       </c>
-      <c r="F20" s="9" t="n">
+      <c r="F20" s="8" t="n">
         <f aca="false">$A$19-E20*$D$19</f>
-        <v>80</v>
+        <v>76.6304347826087</v>
       </c>
       <c r="G20" s="0" t="n">
         <f aca="false">D20*E20+F20</f>
@@ -1255,11 +1261,11 @@
       </c>
       <c r="C21" s="3" t="n">
         <f aca="false">$B$1*($D$1*$H$1-B21*$F$1)/(($D$1+$F$1)*(B21+$H$1))*1000</f>
-        <v>-68.1638552453439</v>
+        <v>-75.74148259767</v>
       </c>
       <c r="D21" s="0" t="n">
         <f aca="false">INT(C21/$J$1)</f>
-        <v>-273</v>
+        <v>-303</v>
       </c>
       <c r="E21" s="6" t="n">
         <f aca="false">($A$22-$A$20)/($D$22-$D$20)</f>
@@ -1267,15 +1273,15 @@
       </c>
       <c r="F21" s="6" t="n">
         <f aca="false">$A$20-E21*$D$20</f>
-        <v>78.9714285714286</v>
+        <v>75.4285714285714</v>
       </c>
       <c r="G21" s="0" t="n">
         <f aca="false">D21*E21+F21</f>
-        <v>110.171428571429</v>
+        <v>110.057142857143</v>
       </c>
       <c r="H21" s="0" t="n">
         <f aca="false">G21-A21</f>
-        <v>0.171428571428578</v>
+        <v>0.0571428571428498</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1287,11 +1293,11 @@
       </c>
       <c r="C22" s="3" t="n">
         <f aca="false">$B$1*($D$1*$H$1-B22*$F$1)/(($D$1+$F$1)*(B22+$H$1))*1000</f>
-        <v>-89.6881541904279</v>
+        <v>-97.2558544189081</v>
       </c>
       <c r="D22" s="5" t="n">
         <f aca="false">INT(C22/$J$1)</f>
-        <v>-359</v>
+        <v>-390</v>
       </c>
       <c r="E22" s="6" t="n">
         <f aca="false">($A$22-$A$20)/($D$22-$D$20)</f>
@@ -1299,7 +1305,7 @@
       </c>
       <c r="F22" s="6" t="n">
         <f aca="false">$A$20-E22*$D$20</f>
-        <v>78.9714285714286</v>
+        <v>75.4285714285714</v>
       </c>
       <c r="G22" s="0" t="n">
         <f aca="false">D22*E22+F22</f>
@@ -1319,27 +1325,27 @@
       </c>
       <c r="C23" s="3" t="n">
         <f aca="false">$B$1*($D$1*$H$1-B23*$F$1)/(($D$1+$F$1)*(B23+$H$1))*1000</f>
-        <v>-110.579730788405</v>
+        <v>-118.135326514556</v>
       </c>
       <c r="D23" s="0" t="n">
         <f aca="false">INT(C23/$J$1)</f>
-        <v>-443</v>
-      </c>
-      <c r="E23" s="9" t="n">
+        <v>-473</v>
+      </c>
+      <c r="E23" s="8" t="n">
         <f aca="false">($A$25-$A$22)/($D$25-$D$22)</f>
-        <v>-0.122950819672131</v>
-      </c>
-      <c r="F23" s="9" t="n">
+        <v>-0.123456790123457</v>
+      </c>
+      <c r="F23" s="8" t="n">
         <f aca="false">$A$22-E23*$D$22</f>
-        <v>75.8606557377049</v>
+        <v>71.8518518518519</v>
       </c>
       <c r="G23" s="0" t="n">
         <f aca="false">D23*E23+F23</f>
-        <v>130.327868852459</v>
+        <v>130.246913580247</v>
       </c>
       <c r="H23" s="0" t="n">
         <f aca="false">G23-A23</f>
-        <v>0.327868852459005</v>
+        <v>0.246913580246911</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1351,27 +1357,27 @@
       </c>
       <c r="C24" s="3" t="n">
         <f aca="false">$B$1*($D$1*$H$1-B24*$F$1)/(($D$1+$F$1)*(B24+$H$1))*1000</f>
-        <v>-130.919249420198</v>
+        <v>-138.460724116028</v>
       </c>
       <c r="D24" s="0" t="n">
         <f aca="false">INT(C24/$J$1)</f>
-        <v>-524</v>
-      </c>
-      <c r="E24" s="9" t="n">
+        <v>-554</v>
+      </c>
+      <c r="E24" s="8" t="n">
         <f aca="false">($A$25-$A$22)/($D$25-$D$22)</f>
-        <v>-0.122950819672131</v>
-      </c>
-      <c r="F24" s="9" t="n">
+        <v>-0.123456790123457</v>
+      </c>
+      <c r="F24" s="8" t="n">
         <f aca="false">$A$22-E24*$D$22</f>
-        <v>75.8606557377049</v>
+        <v>71.8518518518519</v>
       </c>
       <c r="G24" s="0" t="n">
         <f aca="false">D24*E24+F24</f>
-        <v>140.286885245902</v>
+        <v>140.246913580247</v>
       </c>
       <c r="H24" s="0" t="n">
         <f aca="false">G24-A24</f>
-        <v>0.286885245901658</v>
+        <v>0.246913580246911</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1383,19 +1389,19 @@
       </c>
       <c r="C25" s="3" t="n">
         <f aca="false">$B$1*($D$1*$H$1-B25*$F$1)/(($D$1+$F$1)*(B25+$H$1))*1000</f>
-        <v>-150.572300648607</v>
+        <v>-158.097941555501</v>
       </c>
       <c r="D25" s="5" t="n">
         <f aca="false">INT(C25/$J$1)</f>
-        <v>-603</v>
-      </c>
-      <c r="E25" s="9" t="n">
+        <v>-633</v>
+      </c>
+      <c r="E25" s="8" t="n">
         <f aca="false">($A$25-$A$22)/($D$25-$D$22)</f>
-        <v>-0.122950819672131</v>
-      </c>
-      <c r="F25" s="9" t="n">
+        <v>-0.123456790123457</v>
+      </c>
+      <c r="F25" s="8" t="n">
         <f aca="false">$A$22-E25*$D$22</f>
-        <v>75.8606557377049</v>
+        <v>71.8518518518519</v>
       </c>
       <c r="G25" s="0" t="n">
         <f aca="false">D25*E25+F25</f>

</xml_diff>